<commit_message>
added reference for algorithm section
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiankai/Documents/UWaterloo/SYDE644/Literature Review/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiankai/Documents/UWaterloo/SYDE644/SYDE644-Literature-Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA36F88-5E02-BC42-A72D-EFD7CDF63DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6858AFD5-349E-C747-BD5F-D3ED834D16B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{83CC94F4-9313-8E46-9951-0B1C095FD9C9}"/>
   </bookViews>
@@ -351,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +361,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,6 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5A9CDE-8790-C348-8913-5EE9D0C0064C}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,7 +765,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B5" t="s">
@@ -786,7 +793,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B7" t="s">
@@ -941,7 +948,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B20" t="s">
@@ -1075,7 +1082,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B30" t="s">
@@ -1089,7 +1096,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B31" t="s">

</xml_diff>

<commit_message>
fixed small grammatical errors in the paper
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiankai/Documents/UWaterloo/SYDE644/SYDE644-Literature-Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F2DCBC-0A44-7241-8CB9-DECC50656022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF7804D-C79E-BE44-8E2C-5E4C38EA24D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="0" windowWidth="27700" windowHeight="18000" xr2:uid="{83CC94F4-9313-8E46-9951-0B1C095FD9C9}"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="27700" windowHeight="18000" xr2:uid="{83CC94F4-9313-8E46-9951-0B1C095FD9C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5A9CDE-8790-C348-8913-5EE9D0C0064C}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,6 +1206,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>20</v>
       </c>

</xml_diff>